<commit_message>
Start på kranmodell simscape
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sujro\Documents\GitHub\Bachelor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5871003-5798-4C7E-8206-4F1CF4F8DFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA392357-F250-4DF9-8ABA-AF371A063CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{C708630E-46F7-4A85-8DB4-933C05A31E60}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>January</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Explore Simulink</t>
-  </si>
-  <si>
     <t>Explore TwinCat 3</t>
   </si>
   <si>
@@ -126,6 +123,15 @@
   </si>
   <si>
     <t>Setup Github repo</t>
+  </si>
+  <si>
+    <t>Simple crane simscape modell</t>
+  </si>
+  <si>
+    <t>Explore Simscape</t>
+  </si>
+  <si>
+    <t>Set up crane for cylinder force test</t>
   </si>
 </sst>
 </file>
@@ -350,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -366,27 +372,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -396,6 +393,24 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -405,14 +420,11 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -422,11 +434,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFA5D6A7"/>
+      <color rgb="FFEF9A9A"/>
       <color rgb="FFCE93D8"/>
       <color rgb="FF80CBC4"/>
-      <color rgb="FFEF9A9A"/>
       <color rgb="FFFFCC80"/>
-      <color rgb="FFA5D6A7"/>
       <color rgb="FF009688"/>
       <color rgb="FF4CAF50"/>
       <color rgb="FFFF9800"/>
@@ -764,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12C8378-5018-4125-A61A-6AFC813AA3BB}">
   <dimension ref="B3:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -776,36 +788,36 @@
   <sheetData>
     <row r="3" spans="2:21" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="4" spans="2:21" ht="15.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="21" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="18" t="s">
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="21" t="s">
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="20"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="17"/>
     </row>
     <row r="5" spans="2:21" ht="15.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="1">
@@ -871,7 +883,7 @@
     </row>
     <row r="6" spans="2:21" ht="15" x14ac:dyDescent="0.5">
       <c r="B6" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
@@ -895,11 +907,11 @@
     </row>
     <row r="7" spans="2:21" ht="15" x14ac:dyDescent="0.5">
       <c r="B7" s="8"/>
-      <c r="C7" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
+      <c r="C7" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
       <c r="F7" s="8"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -919,11 +931,11 @@
     </row>
     <row r="8" spans="2:21" ht="15" x14ac:dyDescent="0.5">
       <c r="B8" s="8"/>
-      <c r="C8" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
+      <c r="C8" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="8"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -942,10 +954,10 @@
       <c r="U8" s="7"/>
     </row>
     <row r="9" spans="2:21" ht="15" x14ac:dyDescent="0.5">
-      <c r="B9" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="14"/>
+      <c r="B9" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="23"/>
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
@@ -969,8 +981,10 @@
       <c r="B10" s="8"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
+      <c r="E10" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="27"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="7"/>
@@ -988,113 +1002,117 @@
       <c r="U10" s="7"/>
     </row>
     <row r="11" spans="2:21" ht="15.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="17"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="28"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="11"/>
     </row>
     <row r="15" spans="2:21" ht="15" x14ac:dyDescent="0.45">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="2:21" ht="15" x14ac:dyDescent="0.45">
+      <c r="B16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="24"/>
-    </row>
-    <row r="16" spans="2:21" ht="15" x14ac:dyDescent="0.45">
-      <c r="B16" s="25" t="s">
+      <c r="C16" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" spans="2:5" ht="30" x14ac:dyDescent="0.45">
+      <c r="B17" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="26" t="s">
+      <c r="C17" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="25"/>
-    </row>
-    <row r="17" spans="2:5" ht="30" x14ac:dyDescent="0.45">
-      <c r="B17" s="25" t="s">
+      <c r="D17" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="13"/>
+    </row>
+    <row r="18" spans="2:5" ht="15" x14ac:dyDescent="0.45">
+      <c r="B18" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.45">
+      <c r="B19" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="25"/>
-    </row>
-    <row r="18" spans="2:5" ht="15" x14ac:dyDescent="0.45">
-      <c r="B18" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="26" t="s">
+      <c r="C19" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="25"/>
-    </row>
-    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.45">
-      <c r="B19" s="25" t="s">
+      <c r="D19" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="13"/>
+    </row>
+    <row r="20" spans="2:5" ht="30" x14ac:dyDescent="0.45">
+      <c r="B20" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="26" t="s">
+      <c r="C20" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="25"/>
-    </row>
-    <row r="20" spans="2:5" ht="30" x14ac:dyDescent="0.45">
-      <c r="B20" s="25" t="s">
+      <c r="D20" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" spans="2:5" ht="15" x14ac:dyDescent="0.45">
+      <c r="B21" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="26" t="s">
+      <c r="C21" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="25"/>
-    </row>
-    <row r="21" spans="2:5" ht="15" x14ac:dyDescent="0.45">
-      <c r="B21" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="25" t="s">
+      <c r="D21" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="25"/>
+      <c r="E21" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
     <mergeCell ref="R4:U4"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C8:E8"/>

</xml_diff>